<commit_message>
give --> google sheets and removed .picktimes
bug fixed : 'not enough money' situation didn't return
</commit_message>
<xml_diff>
--- a/item.xlsx
+++ b/item.xlsx
@@ -403,7 +403,7 @@
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="7" min="7" width="15.5703125"/>
     <col customWidth="1" max="13" min="13" width="13.140625"/>
@@ -522,7 +522,7 @@
         <v>100</v>
       </c>
       <c r="I2" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>

</xml_diff>